<commit_message>
Proper FOV checking on weapon fire & throw!
</commit_message>
<xml_diff>
--- a/RogueBasin/docs/monster types.xlsx
+++ b/RogueBasin/docs/monster types.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
   <si>
     <t>Random</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>First level</t>
-  </si>
-  <si>
     <t>2nd level</t>
   </si>
   <si>
@@ -231,13 +228,25 @@
     <t>Respond to sound</t>
   </si>
   <si>
-    <t>Introduction to sound</t>
-  </si>
-  <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>Explodes on melee or damage (can damage enemies)</t>
+  </si>
+  <si>
+    <t>Box, no</t>
+  </si>
+  <si>
+    <t>Linear, no</t>
+  </si>
+  <si>
+    <t>First level, non pursue, single hit kills</t>
+  </si>
+  <si>
+    <t>Introduction to sound. Swarmers are a bit easy if they are single hit kills - just find a corridor</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Throw range</t>
   </si>
 </sst>
 </file>
@@ -569,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -582,25 +591,25 @@
     <col min="3" max="4" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="39.140625" customWidth="1"/>
+    <col min="7" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -609,27 +618,30 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -637,22 +649,22 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -660,86 +672,86 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>33</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="C10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="C12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>32</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -750,28 +762,31 @@
       <c r="G14">
         <v>2</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
         <v>33</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>34</v>
       </c>
-      <c r="K14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -782,65 +797,63 @@
       <c r="G15">
         <v>2</v>
       </c>
-      <c r="I15" t="s">
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="J15" t="s">
         <v>33</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>34</v>
       </c>
-      <c r="K15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>33</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>34</v>
       </c>
-      <c r="K17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
         <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" t="s">
-        <v>40</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -848,16 +861,19 @@
       <c r="G19">
         <v>2</v>
       </c>
-      <c r="I19" t="s">
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="J19" t="s">
         <v>33</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -866,7 +882,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -877,24 +893,24 @@
       <c r="G21">
         <v>4</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>23</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>28</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="s">
-        <v>47</v>
       </c>
       <c r="B24">
         <v>5</v>
@@ -903,10 +919,10 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
@@ -914,19 +930,19 @@
       <c r="G24">
         <v>3</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>33</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>27</v>
       </c>
-      <c r="K24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -935,30 +951,30 @@
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G25">
         <v>3</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>33</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>27</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" t="s">
-        <v>55</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -967,33 +983,33 @@
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G27">
         <v>5</v>
       </c>
-      <c r="H27" t="s">
-        <v>73</v>
-      </c>
       <c r="I27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" t="s">
         <v>22</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>34</v>
       </c>
-      <c r="K27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -1002,41 +1018,47 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" t="s">
         <v>42</v>
       </c>
-      <c r="H29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" t="s">
-        <v>43</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
         <v>57</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
         <v>58</v>
-      </c>
-      <c r="C34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>59</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1045,9 +1067,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -1058,33 +1080,48 @@
       <c r="D37" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="F37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D38" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
         <v>66</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>67</v>
-      </c>
-      <c r="C39" t="s">
-        <v>68</v>
       </c>
       <c r="D39" t="s">
         <v>28</v>
+      </c>
+      <c r="E39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>